<commit_message>
variable weightage and baskets
</commit_message>
<xml_diff>
--- a/Master R&D.xlsx
+++ b/Master R&D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AKSHAT\internship_clone\mastering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97703B9A-69EF-4768-AAF2-7C29E85EF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AF8A46-9D2E-46F9-9DA6-7AEA8F912126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="keycap" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="jeetprk" sheetId="11" r:id="rId11"/>
     <sheet name="umang" sheetId="12" r:id="rId12"/>
     <sheet name="chetan" sheetId="13" r:id="rId13"/>
-    <sheet name="akshatshah" sheetId="14" r:id="rId14"/>
+    <sheet name="akshat" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">kaushal!$A$1:$G$22</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="65">
   <si>
     <t>Strategy</t>
   </si>
@@ -228,7 +228,7 @@
     <t>home</t>
   </si>
   <si>
-    <t>akshatshah</t>
+    <t>akshat</t>
   </si>
   <si>
     <t>Total</t>
@@ -238,7 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,11 +279,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,27 +288,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -337,14 +317,20 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -352,9 +338,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -641,27 +624,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="9" customWidth="1"/>
+    <col min="7" max="12" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -673,40 +667,28 @@
         <f>E42*C2/100</f>
         <v>434384.18599999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>7.9</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E41" si="0">B2/F2</f>
+      <c r="E2" s="1">
+        <f>B2/F2</f>
         <v>217192.09299999999</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <f>E42*C3/100</f>
-        <v>434384.18599999999</v>
-      </c>
-      <c r="C3">
-        <v>7.9</v>
-      </c>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="E3" s="1">
+        <f>B2/F2</f>
         <v>217192.09299999999</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -717,150 +699,78 @@
         <f>E42*C4/100</f>
         <v>1990469.3080000002</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>36.200000000000003</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="E4" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <f>E42*C5/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C5">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="E5" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <f>E42*C6/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C6">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E6" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <f>E42*C7/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C7">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="E7" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>E42*C8/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C8">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="E8" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <f>E42*C9/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C9">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
+      <c r="E9" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
       </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f>E42*C10/100</f>
-        <v>1990469.3080000002</v>
-      </c>
-      <c r="C10">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
+      <c r="E10" s="1">
+        <f>B4/F4</f>
         <v>284352.75828571431</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,150 +781,78 @@
         <f>E42*C11/100</f>
         <v>951246.38199999998</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>17.3</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
+      <c r="E11" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <f>E42*C12/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C12">
-        <v>17.3</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
+      <c r="E12" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <f>E42*C13/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C13">
-        <v>17.3</v>
-      </c>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
+      <c r="E13" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F13">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <f>E42*C14/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C14">
-        <v>17.3</v>
-      </c>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
+      <c r="E14" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <f>E42*C15/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C15">
-        <v>17.3</v>
-      </c>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
+      <c r="E15" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <f>E42*C16/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C16">
-        <v>17.3</v>
-      </c>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
+      <c r="E16" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
       </c>
-      <c r="F16">
-        <v>7</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <f>E42*C17/100</f>
-        <v>951246.38199999998</v>
-      </c>
-      <c r="C17">
-        <v>17.3</v>
-      </c>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="E17" s="1">
+        <f>B11/F11</f>
         <v>135892.34028571428</v>
-      </c>
-      <c r="F17">
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1025,84 +863,48 @@
         <f>E42*C18/100</f>
         <v>285923.76799999998</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="E18" s="1">
+        <f>B18/F18</f>
         <v>71480.941999999995</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <f>E42*C19/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C19">
-        <v>5.2</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="E19" s="1">
+        <f>B18/F18</f>
         <v>71480.941999999995</v>
       </c>
-      <c r="F19">
-        <v>4</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <f>E42*C20/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C20">
-        <v>5.2</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="E20" s="1">
+        <f>B18/F18</f>
         <v>71480.941999999995</v>
       </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <f>E42*C21/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C21">
-        <v>5.2</v>
-      </c>
+      <c r="C21" s="7"/>
       <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E21" s="1">
+        <f>B18/F18</f>
         <v>71480.941999999995</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1113,128 +915,68 @@
         <f>E42*C22/100</f>
         <v>313416.43800000002</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>5.7</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="E22" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <f>E42*C23/100</f>
-        <v>313416.43800000002</v>
-      </c>
-      <c r="C23">
-        <v>5.7</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" t="s">
         <v>32</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="E23" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
       </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <f>E42*C24/100</f>
-        <v>313416.43800000002</v>
-      </c>
-      <c r="C24">
-        <v>5.7</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
+      <c r="E24" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
       </c>
-      <c r="F24">
-        <v>6</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
-        <f>E42*C25/100</f>
-        <v>313416.43800000002</v>
-      </c>
-      <c r="C25">
-        <v>5.7</v>
-      </c>
+      <c r="C25" s="7"/>
       <c r="D25" t="s">
         <v>32</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
+      <c r="E25" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
       </c>
-      <c r="F25">
-        <v>6</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <f>E42*C26/100</f>
-        <v>313416.43800000002</v>
-      </c>
-      <c r="C26">
-        <v>5.7</v>
-      </c>
+      <c r="C26" s="7"/>
       <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
+      <c r="E26" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
       </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <f>E42*C27/100</f>
-        <v>313416.43800000002</v>
-      </c>
-      <c r="C27">
-        <v>5.7</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="E27" s="1">
+        <f>B22/F22</f>
         <v>52236.073000000004</v>
-      </c>
-      <c r="F27">
-        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1245,150 +987,78 @@
         <f>E42*C28/100</f>
         <v>285923.76799999998</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>5.2</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
+      <c r="E28" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29">
-        <f>E42*C29/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C29">
-        <v>5.2</v>
-      </c>
+      <c r="C29" s="7"/>
       <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
+      <c r="E29" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <f>E42*C30/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C30">
-        <v>5.2</v>
-      </c>
+      <c r="C30" s="7"/>
       <c r="D30" t="s">
         <v>12</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
+      <c r="E30" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31">
-        <f>E42*C31/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C31">
-        <v>5.2</v>
-      </c>
+      <c r="C31" s="7"/>
       <c r="D31" t="s">
         <v>36</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
+      <c r="E31" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F31">
-        <v>7</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <f>E42*C32/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C32">
-        <v>5.2</v>
-      </c>
+      <c r="C32" s="7"/>
       <c r="D32" t="s">
         <v>37</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
+      <c r="E32" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F32">
-        <v>7</v>
-      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33">
-        <f>E42*C33/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C33">
-        <v>5.2</v>
-      </c>
+      <c r="C33" s="7"/>
       <c r="D33" t="s">
         <v>38</v>
       </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
+      <c r="E33" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
       </c>
-      <c r="F33">
-        <v>7</v>
-      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <f>E42*C34/100</f>
-        <v>285923.76799999998</v>
-      </c>
-      <c r="C34">
-        <v>5.2</v>
-      </c>
+      <c r="C34" s="7"/>
       <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
+      <c r="E34" s="1">
+        <f>B28/F28</f>
         <v>40846.252571428566</v>
-      </c>
-      <c r="F34">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1399,59 +1069,35 @@
         <f>E42*C35/100</f>
         <v>170454.55400000003</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="7">
         <v>3.1</v>
       </c>
       <c r="D35" t="s">
         <v>41</v>
       </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
+      <c r="E35" s="1">
+        <f>B35/F35</f>
         <v>56818.184666666675</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <f>E42*C36/100</f>
-        <v>170454.55400000003</v>
-      </c>
-      <c r="C36">
-        <v>3.1</v>
-      </c>
+      <c r="C36" s="7"/>
       <c r="D36" t="s">
         <v>42</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
+      <c r="E36" s="1">
+        <f>B35/F35</f>
         <v>56818.184666666675</v>
       </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <f>E42*C37/100</f>
-        <v>170454.55400000003</v>
-      </c>
-      <c r="C37">
-        <v>3.1</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
+      <c r="C37" s="7"/>
+      <c r="E37" s="1">
+        <f>B35/F35</f>
         <v>56818.184666666675</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1462,17 +1108,17 @@
         <f>E42*C38/100</f>
         <v>120967.74800000001</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="7">
         <v>2.2000000000000002</v>
       </c>
       <c r="D38" t="s">
         <v>44</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
+      <c r="E38" s="1">
+        <f>B38/F38</f>
         <v>120967.74800000001</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1484,62 +1130,38 @@
         <f>E42*C39/100</f>
         <v>428885.65199999994</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="7">
         <v>7.8</v>
       </c>
       <c r="D39" t="s">
         <v>46</v>
       </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
+      <c r="E39" s="1">
+        <f>B39/F39</f>
         <v>142961.88399999999</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40">
-        <f>E42*C40/100</f>
-        <v>428885.65199999994</v>
-      </c>
-      <c r="C40">
-        <v>7.8</v>
-      </c>
+      <c r="C40" s="7"/>
       <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
+      <c r="E40" s="1">
+        <f>B39/F39</f>
         <v>142961.88399999999</v>
       </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <f>E42*C41/100</f>
-        <v>428885.65199999994</v>
-      </c>
-      <c r="C41">
-        <v>7.8</v>
-      </c>
+      <c r="C41" s="7"/>
       <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
+      <c r="E41" s="1">
+        <f>B39/F39</f>
         <v>142961.88399999999</v>
-      </c>
-      <c r="F41">
-        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1551,7 +1173,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1567,7 +1190,7 @@
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
     <col min="7" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1587,7 +1210,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1599,7 +1222,7 @@
         <f>E19*C2/100</f>
         <v>272467.08199999999</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>10.9</v>
       </c>
       <c r="D2" t="s">
@@ -1614,7 +1237,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -1628,7 +1251,7 @@
         <f>E19*C4/100</f>
         <v>1244849.6039999998</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>49.8</v>
       </c>
       <c r="D4" t="s">
@@ -1643,7 +1266,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -1653,7 +1276,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -1663,7 +1286,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1296,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -1683,7 +1306,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -1693,7 +1316,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -1710,7 +1333,7 @@
         <f>E19*C11</f>
         <v>59492812.399999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>23.8</v>
       </c>
       <c r="D11" t="s">
@@ -1725,7 +1348,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1358,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
@@ -1745,7 +1368,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -1755,7 +1378,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -1765,7 +1388,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -1775,7 +1398,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -1792,7 +1415,7 @@
         <f>E19*C18</f>
         <v>7749063.7999999998</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>3.1</v>
       </c>
       <c r="D18" t="s">
@@ -1802,7 +1425,7 @@
         <f>B18/F18</f>
         <v>7749063.7999999998</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>1</v>
       </c>
     </row>
@@ -1831,7 +1454,7 @@
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
     <col min="7" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1851,7 +1474,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1988,7 +1611,7 @@
         <f>B11/F11</f>
         <v>65055.218999999997</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2015,7 +1638,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -2034,7 +1657,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2046,7 +1669,7 @@
         <f>E15*C2/100</f>
         <v>403237.15199999994</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>17.7</v>
       </c>
       <c r="D2" t="s">
@@ -2056,12 +1679,12 @@
         <f>B2/F2</f>
         <v>201618.57599999997</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +1701,7 @@
         <f>E15*C4/100</f>
         <v>881654.11200000008</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>38.700000000000003</v>
       </c>
       <c r="D4" t="s">
@@ -2088,12 +1711,12 @@
         <f>B4/F4</f>
         <v>125950.58742857144</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>19</v>
       </c>
@@ -2103,7 +1726,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>20</v>
       </c>
@@ -2113,7 +1736,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>21</v>
       </c>
@@ -2123,7 +1746,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>22</v>
       </c>
@@ -2133,7 +1756,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>23</v>
       </c>
@@ -2143,7 +1766,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>24</v>
       </c>
@@ -2160,7 +1783,7 @@
         <f>E15*C11/100</f>
         <v>113908.8</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>5</v>
       </c>
       <c r="D11" t="s">
@@ -2170,7 +1793,7 @@
         <f>B11/F11</f>
         <v>113908.8</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="9">
         <v>1</v>
       </c>
     </row>
@@ -2182,7 +1805,7 @@
         <f>E15*C12/100</f>
         <v>398680.8</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>17.5</v>
       </c>
       <c r="D12" t="s">
@@ -2192,12 +1815,12 @@
         <f>B12/F12</f>
         <v>132893.6</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>46</v>
       </c>
@@ -2207,7 +1830,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>47</v>
       </c>
@@ -2233,7 +1856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -2241,7 +1864,7 @@
   <cols>
     <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="8.88671875" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
     <col min="7" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2261,7 +1884,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2273,7 +1896,7 @@
         <f>E8*C2/100</f>
         <v>490048.24799999996</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>28.4</v>
       </c>
       <c r="D2" t="s">
@@ -2283,12 +1906,12 @@
         <f>B2/F2</f>
         <v>245024.12399999998</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -2306,7 +1929,7 @@
         <f>E8*C4/100</f>
         <v>139767.28200000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>8.1</v>
       </c>
       <c r="D4" t="s">
@@ -2316,7 +1939,7 @@
         <f>B4/F4</f>
         <v>139767.28200000001</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="9">
         <v>1</v>
       </c>
       <c r="H4" s="4"/>
@@ -2330,7 +1953,7 @@
         <f>E8*C5/100</f>
         <v>484871.68200000003</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>28.1</v>
       </c>
       <c r="D5" t="s">
@@ -2340,14 +1963,14 @@
         <f>B5/F5</f>
         <v>161623.894</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="10">
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>46</v>
       </c>
@@ -2359,7 +1982,7 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>47</v>
       </c>
@@ -2425,93 +2048,93 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B2">
-        <f>E7*C2/100</f>
-        <v>79000</v>
+        <f>E6*C2/100</f>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>790</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <f>B2/F2</f>
-        <v>39500</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <f>E7*C3/100</f>
-        <v>79000</v>
+        <f>E6*C3/100</f>
+        <v>40</v>
       </c>
       <c r="C3">
-        <v>790</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="E3">
         <f>B3/F3</f>
-        <v>39500</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <f>E6*C4/100</f>
         <v>40</v>
       </c>
-      <c r="B4">
-        <f>E7*C4/100</f>
-        <v>31000</v>
-      </c>
       <c r="C4">
-        <v>310</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <f>B4/F4</f>
-        <v>10333.333333333334</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -2519,21 +2142,21 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <f>E6*C5/100</f>
         <v>40</v>
       </c>
-      <c r="B5">
-        <f>E7*C5/100</f>
-        <v>31000</v>
-      </c>
       <c r="C5">
-        <v>310</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E5">
         <f>B5/F5</f>
-        <v>10333.333333333334</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -2541,29 +2164,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <f>E7*C6/100</f>
-        <v>31000</v>
-      </c>
-      <c r="C6">
-        <v>310</v>
+        <v>64</v>
       </c>
       <c r="E6">
-        <f>B6/F6</f>
-        <v>10333.333333333334</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7">
-        <v>10000</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2573,7 +2177,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
@@ -2582,34 +2186,34 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3002,7 +2606,7 @@
         <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
@@ -3020,13 +2624,77 @@
         <v>52</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="I14" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3049,7 +2717,7 @@
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3068,7 +2736,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3080,7 +2748,7 @@
         <f>E22*C2/100</f>
         <v>294000.00000000006</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>9.8000000000000007</v>
       </c>
       <c r="D2" t="s">
@@ -3095,7 +2763,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -3112,7 +2780,7 @@
         <f>E22*C4/100</f>
         <v>1341000.0000000002</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>44.7</v>
       </c>
       <c r="D4" t="s">
@@ -3127,7 +2795,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -3137,7 +2805,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -3147,7 +2815,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -3157,7 +2825,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -3167,7 +2835,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -3177,7 +2845,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -3194,7 +2862,7 @@
         <f>E22*C11/100</f>
         <v>641999.99999999988</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>21.4</v>
       </c>
       <c r="D11" t="s">
@@ -3209,7 +2877,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -3219,7 +2887,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
@@ -3229,7 +2897,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -3239,7 +2907,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -3249,7 +2917,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -3259,7 +2927,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -3276,7 +2944,7 @@
         <f>E22*C18/100</f>
         <v>84000</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>2.8</v>
       </c>
       <c r="D18" t="s">
@@ -3286,7 +2954,7 @@
         <f>B18/F18</f>
         <v>84000</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>1</v>
       </c>
     </row>
@@ -3298,7 +2966,7 @@
         <f>E22*C19/100</f>
         <v>291000.00000000006</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>9.7000000000000011</v>
       </c>
       <c r="D19" t="s">
@@ -3313,7 +2981,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="D20" t="s">
         <v>46</v>
       </c>
@@ -3323,7 +2991,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
+      <c r="C21" s="7"/>
       <c r="D21" t="s">
         <v>47</v>
       </c>
@@ -3357,7 +3025,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3376,7 +3044,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3388,7 +3056,7 @@
         <f>E18*C2/100</f>
         <v>169691.2</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>11.2</v>
       </c>
       <c r="D2" t="s">
@@ -3398,12 +3066,12 @@
         <f>B2/F2</f>
         <v>84845.6</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -3420,7 +3088,7 @@
         <f>E18*C4/100</f>
         <v>778761.4</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>51.4</v>
       </c>
       <c r="D4" t="s">
@@ -3430,12 +3098,12 @@
         <f>B4/F4</f>
         <v>111251.62857142858</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -3445,7 +3113,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -3455,7 +3123,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -3465,7 +3133,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -3475,7 +3143,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -3485,7 +3153,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -3502,7 +3170,7 @@
         <f>E18*C11/100</f>
         <v>372714.6</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>24.6</v>
       </c>
       <c r="D11" t="s">
@@ -3512,12 +3180,12 @@
         <f>B11/F11</f>
         <v>53244.942857142851</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -3527,7 +3195,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
@@ -3537,7 +3205,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -3547,7 +3215,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -3557,7 +3225,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -3567,7 +3235,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -3600,7 +3268,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3619,7 +3287,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3631,7 +3299,7 @@
         <f>E11*C2/100</f>
         <v>211199.20704999997</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>31.3</v>
       </c>
       <c r="D2" t="s">
@@ -3646,7 +3314,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -3663,7 +3331,7 @@
         <f>E11*C4/100</f>
         <v>463558.64295000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>68.7</v>
       </c>
       <c r="D4" t="s">
@@ -3678,7 +3346,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>19</v>
       </c>
@@ -3688,7 +3356,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>20</v>
       </c>
@@ -3698,7 +3366,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>21</v>
       </c>
@@ -3708,7 +3376,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>22</v>
       </c>
@@ -3718,7 +3386,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>23</v>
       </c>
@@ -3728,7 +3396,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>24</v>
       </c>
@@ -3746,7 +3414,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
+      <c r="B12" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3763,7 +3431,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -3782,7 +3450,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3794,7 +3462,7 @@
         <f>E19*C2/100</f>
         <v>241053.71799999999</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>10.9</v>
       </c>
       <c r="D2" t="s">
@@ -3809,7 +3477,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -3826,7 +3494,7 @@
         <f>E19*C4/100</f>
         <v>1101327.996</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>49.8</v>
       </c>
       <c r="D4" t="s">
@@ -3841,7 +3509,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -3851,7 +3519,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -3861,7 +3529,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -3871,7 +3539,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -3881,7 +3549,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -3891,7 +3559,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -3908,7 +3576,7 @@
         <f>E19*C11/100</f>
         <v>526337.47600000002</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>23.8</v>
       </c>
       <c r="D11" t="s">
@@ -3923,7 +3591,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -3933,7 +3601,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
@@ -3943,7 +3611,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -3953,7 +3621,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -3963,7 +3631,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -3973,7 +3641,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -3990,7 +3658,7 @@
         <f>E19*C18/100</f>
         <v>685565.62</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>31</v>
       </c>
       <c r="D18" t="s">
@@ -4000,7 +3668,7 @@
         <f>B18/F18</f>
         <v>685565.62</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4027,7 +3695,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4047,7 +3715,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4059,7 +3727,7 @@
         <f>E11*C2/100</f>
         <v>293928.28400000004</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>31.3</v>
       </c>
       <c r="D2" t="s">
@@ -4074,7 +3742,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -4091,7 +3759,7 @@
         <f>E11*C4/100</f>
         <v>645139.71600000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>68.7</v>
       </c>
       <c r="D4" t="s">
@@ -4200,7 +3868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4219,7 +3887,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4231,7 +3899,7 @@
         <f>E29*C2/100</f>
         <v>3172400</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <v>10.3</v>
       </c>
       <c r="D2" t="s">
@@ -4241,12 +3909,12 @@
         <f>B2/F2</f>
         <v>1586200</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
@@ -4263,7 +3931,7 @@
         <f>E29*C4/100</f>
         <v>14537600</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>47.2</v>
       </c>
       <c r="D4" t="s">
@@ -4273,12 +3941,12 @@
         <f>B4/F4</f>
         <v>2076800</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
@@ -4288,7 +3956,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
@@ -4298,7 +3966,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
@@ -4308,7 +3976,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
@@ -4318,7 +3986,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="6"/>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
@@ -4328,7 +3996,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -4345,7 +4013,7 @@
         <f>E29*C11/100</f>
         <v>6960800</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>22.6</v>
       </c>
       <c r="D11" t="s">
@@ -4355,12 +4023,12 @@
         <f>B11/F11</f>
         <v>994400</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
@@ -4370,7 +4038,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" s="6"/>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
@@ -4380,7 +4048,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
@@ -4390,7 +4058,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -4400,7 +4068,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -4410,7 +4078,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C17" s="6"/>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -4427,7 +4095,7 @@
         <f>E29*C18/100</f>
         <v>2094400</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>6.8</v>
       </c>
       <c r="D18" t="s">
@@ -4437,12 +4105,12 @@
         <f>B18/F18</f>
         <v>299200</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="10">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="6"/>
+      <c r="C19" s="7"/>
       <c r="D19" t="s">
         <v>16</v>
       </c>
@@ -4452,7 +4120,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
+      <c r="C20" s="7"/>
       <c r="D20" t="s">
         <v>12</v>
       </c>
@@ -4462,7 +4130,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="6"/>
+      <c r="C21" s="7"/>
       <c r="D21" t="s">
         <v>36</v>
       </c>
@@ -4472,7 +4140,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C22" s="6"/>
+      <c r="C22" s="7"/>
       <c r="D22" t="s">
         <v>37</v>
       </c>
@@ -4482,7 +4150,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C23" s="6"/>
+      <c r="C23" s="7"/>
       <c r="D23" t="s">
         <v>38</v>
       </c>
@@ -4492,7 +4160,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
+      <c r="C24" s="7"/>
       <c r="D24" t="s">
         <v>39</v>
       </c>
@@ -4509,7 +4177,7 @@
         <f>E29*C25/100</f>
         <v>893200</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>2.9</v>
       </c>
       <c r="D25" t="s">
@@ -4519,7 +4187,7 @@
         <f>B25/F25</f>
         <v>893200</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="9">
         <v>1</v>
       </c>
     </row>
@@ -4531,7 +4199,7 @@
         <f>E29*C26/100</f>
         <v>3141600</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="7">
         <v>10.199999999999999</v>
       </c>
       <c r="D26" t="s">
@@ -4541,12 +4209,12 @@
         <f>B26/F26</f>
         <v>1047200</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C27" s="6"/>
+      <c r="C27" s="7"/>
       <c r="D27" t="s">
         <v>46</v>
       </c>
@@ -4556,7 +4224,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
+      <c r="C28" s="7"/>
       <c r="D28" t="s">
         <v>47</v>
       </c>
@@ -4582,27 +4250,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="8" customWidth="1"/>
+    <col min="7" max="13" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -4614,40 +4293,28 @@
         <f>E42*C2/100</f>
         <v>917629.39799999993</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="7">
         <v>7.9</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
-        <f t="shared" ref="E2:E41" si="0">B2/F2</f>
+      <c r="E2" s="1">
+        <f>B2/F2</f>
         <v>458814.69899999996</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <f>E42*C3/100</f>
-        <v>917629.39799999993</v>
-      </c>
-      <c r="C3">
-        <v>7.9</v>
-      </c>
+      <c r="C3" s="7"/>
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="E3" s="1">
+        <f>B2/F2</f>
         <v>458814.69899999996</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4658,150 +4325,78 @@
         <f>E42*C4/100</f>
         <v>4204833.4440000001</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <v>36.200000000000003</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
+      <c r="E4" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <f>E42*C5/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C5">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
+      <c r="E5" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <f>E42*C6/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C6">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
+      <c r="E6" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <f>E42*C7/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C7">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C7" s="7"/>
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
+      <c r="E7" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>E42*C8/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C8">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C8" s="7"/>
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
+      <c r="E8" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <f>E42*C9/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C9">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C9" s="7"/>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
+      <c r="E9" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
       </c>
-      <c r="F9">
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <f>E42*C10/100</f>
-        <v>4204833.4440000001</v>
-      </c>
-      <c r="C10">
-        <v>36.200000000000003</v>
-      </c>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
+      <c r="E10" s="1">
+        <f>B4/F4</f>
         <v>600690.49199999997</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -4812,150 +4407,78 @@
         <f>E42*C11/100</f>
         <v>2009492.226</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>17.3</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
+      <c r="E11" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12">
-        <f>E42*C12/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C12">
-        <v>17.3</v>
-      </c>
+      <c r="C12" s="7"/>
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
+      <c r="E12" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <f>E42*C13/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C13">
-        <v>17.3</v>
-      </c>
+      <c r="C13" s="7"/>
       <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
+      <c r="E13" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F13">
-        <v>7</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <f>E42*C14/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C14">
-        <v>17.3</v>
-      </c>
+      <c r="C14" s="7"/>
       <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
+      <c r="E14" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F14">
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
-        <f>E42*C15/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C15">
-        <v>17.3</v>
-      </c>
+      <c r="C15" s="7"/>
       <c r="D15" t="s">
         <v>22</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
+      <c r="E15" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <f>E42*C16/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C16">
-        <v>17.3</v>
-      </c>
+      <c r="C16" s="7"/>
       <c r="D16" t="s">
         <v>23</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
+      <c r="E16" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
       </c>
-      <c r="F16">
-        <v>7</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <f>E42*C17/100</f>
-        <v>2009492.226</v>
-      </c>
-      <c r="C17">
-        <v>17.3</v>
-      </c>
+      <c r="C17" s="7"/>
       <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="E17" s="1">
+        <f>B11/F11</f>
         <v>287070.31800000003</v>
-      </c>
-      <c r="F17">
-        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -4966,84 +4489,48 @@
         <f>E42*C18/100</f>
         <v>604009.22399999993</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>5.2</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="E18" s="1">
+        <f>B18/F18</f>
         <v>151002.30599999998</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19">
-        <f>E42*C19/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C19">
-        <v>5.2</v>
-      </c>
+      <c r="C19" s="7"/>
       <c r="D19" t="s">
         <v>27</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="E19" s="1">
+        <f>B18/F18</f>
         <v>151002.30599999998</v>
       </c>
-      <c r="F19">
-        <v>4</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
-        <f>E42*C20/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C20">
-        <v>5.2</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
+      <c r="E20" s="1">
+        <f>B18/F18</f>
         <v>151002.30599999998</v>
       </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <f>E42*C21/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C21">
-        <v>5.2</v>
-      </c>
+      <c r="C21" s="7"/>
       <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E21" s="1">
+        <f>B18/F18</f>
         <v>151002.30599999998</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -5054,128 +4541,68 @@
         <f>E42*C22/100</f>
         <v>662087.03399999999</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>5.7</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
+      <c r="E22" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <f>E42*C23/100</f>
-        <v>662087.03399999999</v>
-      </c>
-      <c r="C23">
-        <v>5.7</v>
-      </c>
+      <c r="C23" s="7"/>
       <c r="D23" t="s">
         <v>32</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
+      <c r="E23" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
       </c>
-      <c r="F23">
-        <v>6</v>
-      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <f>E42*C24/100</f>
-        <v>662087.03399999999</v>
-      </c>
-      <c r="C24">
-        <v>5.7</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" t="s">
         <v>32</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
+      <c r="E24" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
       </c>
-      <c r="F24">
-        <v>6</v>
-      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
-        <f>E42*C25/100</f>
-        <v>662087.03399999999</v>
-      </c>
-      <c r="C25">
-        <v>5.7</v>
-      </c>
+      <c r="C25" s="7"/>
       <c r="D25" t="s">
         <v>32</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
+      <c r="E25" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
       </c>
-      <c r="F25">
-        <v>6</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <f>E42*C26/100</f>
-        <v>662087.03399999999</v>
-      </c>
-      <c r="C26">
-        <v>5.7</v>
-      </c>
+      <c r="C26" s="7"/>
       <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
+      <c r="E26" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
       </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B27">
-        <f>E42*C27/100</f>
-        <v>662087.03399999999</v>
-      </c>
-      <c r="C27">
-        <v>5.7</v>
-      </c>
+      <c r="C27" s="7"/>
       <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="E27" s="1">
+        <f>B22/F22</f>
         <v>110347.83899999999</v>
-      </c>
-      <c r="F27">
-        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -5186,150 +4613,78 @@
         <f>E42*C28/100</f>
         <v>604009.22399999993</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>5.2</v>
       </c>
       <c r="D28" t="s">
         <v>35</v>
       </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
+      <c r="E28" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29">
-        <f>E42*C29/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C29">
-        <v>5.2</v>
-      </c>
+      <c r="C29" s="7"/>
       <c r="D29" t="s">
         <v>16</v>
       </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
+      <c r="E29" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F29">
-        <v>7</v>
-      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <f>E42*C30/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C30">
-        <v>5.2</v>
-      </c>
+      <c r="C30" s="7"/>
       <c r="D30" t="s">
         <v>12</v>
       </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
+      <c r="E30" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F30">
-        <v>7</v>
-      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31">
-        <f>E42*C31/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C31">
-        <v>5.2</v>
-      </c>
+      <c r="C31" s="7"/>
       <c r="D31" t="s">
         <v>36</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
+      <c r="E31" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F31">
-        <v>7</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32">
-        <f>E42*C32/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C32">
-        <v>5.2</v>
-      </c>
+      <c r="C32" s="7"/>
       <c r="D32" t="s">
         <v>37</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
+      <c r="E32" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F32">
-        <v>7</v>
-      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33">
-        <f>E42*C33/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C33">
-        <v>5.2</v>
-      </c>
+      <c r="C33" s="7"/>
       <c r="D33" t="s">
         <v>38</v>
       </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
+      <c r="E33" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
       </c>
-      <c r="F33">
-        <v>7</v>
-      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <f>E42*C34/100</f>
-        <v>604009.22399999993</v>
-      </c>
-      <c r="C34">
-        <v>5.2</v>
-      </c>
+      <c r="C34" s="7"/>
       <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
+      <c r="E34" s="1">
+        <f>B28/F28</f>
         <v>86287.031999999992</v>
-      </c>
-      <c r="F34">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5340,59 +4695,35 @@
         <f>E42*C35/100</f>
         <v>360082.42200000002</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="7">
         <v>3.1</v>
       </c>
       <c r="D35" t="s">
         <v>41</v>
       </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
+      <c r="E35" s="1">
+        <f>B35/F35</f>
         <v>120027.474</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <f>E42*C36/100</f>
-        <v>360082.42200000002</v>
-      </c>
-      <c r="C36">
-        <v>3.1</v>
-      </c>
+      <c r="C36" s="7"/>
       <c r="D36" t="s">
         <v>42</v>
       </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
+      <c r="E36" s="1">
+        <f>B35/F35</f>
         <v>120027.474</v>
       </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37">
-        <f>E42*C37/100</f>
-        <v>360082.42200000002</v>
-      </c>
-      <c r="C37">
-        <v>3.1</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
+      <c r="C37" s="7"/>
+      <c r="E37" s="1">
+        <f>B35/F35</f>
         <v>120027.474</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -5403,17 +4734,17 @@
         <f>E42*C38/100</f>
         <v>255542.36400000003</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="7">
         <v>2.2000000000000002</v>
       </c>
       <c r="D38" t="s">
         <v>44</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
+      <c r="E38" s="1">
+        <f>B38/F38</f>
         <v>255542.36400000003</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="6">
         <v>1</v>
       </c>
     </row>
@@ -5425,62 +4756,38 @@
         <f>E42*C39/100</f>
         <v>906013.83599999989</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="7">
         <v>7.8</v>
       </c>
       <c r="D39" t="s">
         <v>46</v>
       </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
+      <c r="E39" s="1">
+        <f>B39/F39</f>
         <v>302004.61199999996</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40">
-        <f>E42*C40/100</f>
-        <v>906013.83599999989</v>
-      </c>
-      <c r="C40">
-        <v>7.8</v>
-      </c>
+      <c r="C40" s="7"/>
       <c r="D40" t="s">
         <v>46</v>
       </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
+      <c r="E40" s="1">
+        <f>B39/F39</f>
         <v>302004.61199999996</v>
       </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <f>E42*C41/100</f>
-        <v>906013.83599999989</v>
-      </c>
-      <c r="C41">
-        <v>7.8</v>
-      </c>
+      <c r="C41" s="7"/>
       <c r="D41" t="s">
         <v>47</v>
       </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
+      <c r="E41" s="1">
+        <f>B39/F39</f>
         <v>302004.61199999996</v>
-      </c>
-      <c r="F41">
-        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -5492,6 +4799,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>